<commit_message>
🔨Aba Lateral (falta o js)
</commit_message>
<xml_diff>
--- a/Database Placeholders.xlsx
+++ b/Database Placeholders.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/dfb5b4737cec9096/Desktop/Programação/TCC/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="175" documentId="8_{46F3AB83-DCBD-4553-86B5-EFDF33352B99}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{28B29817-6022-47C7-BA51-3B1FA5502EFC}"/>
+  <xr:revisionPtr revIDLastSave="178" documentId="8_{46F3AB83-DCBD-4553-86B5-EFDF33352B99}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{9A4DAEE2-0EFA-4F92-AF7D-97682AA2E806}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{0C260EFA-34F1-469A-9DCE-051C064AD26C}"/>
   </bookViews>
@@ -512,9 +512,6 @@
     <t>'899.00'),</t>
   </si>
   <si>
-    <t>(' Brinco clássico de ouro amarelo, ótimo para celebrações especiais.',</t>
-  </si>
-  <si>
     <t>'Brinco de Prata com Pérola',</t>
   </si>
   <si>
@@ -533,18 +530,12 @@
     <t>'1499.00'),</t>
   </si>
   <si>
-    <t>(' Brinco romântico de ouro rosé, perfeito para ocasiões especiais.',</t>
-  </si>
-  <si>
     <t>'Brinco de Prata com Topázio',</t>
   </si>
   <si>
     <t>'349.00'),</t>
   </si>
   <si>
-    <t>(' Brinco delicado de prata com topázio, ótimo para eventos formais.',</t>
-  </si>
-  <si>
     <t>'Brinco de Titânio',</t>
   </si>
   <si>
@@ -657,6 +648,15 @@
   </si>
   <si>
     <t>'399.90'),</t>
+  </si>
+  <si>
+    <t>('Brinco romântico de ouro rosé, perfeito para ocasiões especiais.',</t>
+  </si>
+  <si>
+    <t>('Brinco delicado de prata com topázio, ótimo para eventos formais.',</t>
+  </si>
+  <si>
+    <t>('Brinco clássico de ouro amarelo, ótimo para celebrações especiais.',</t>
   </si>
 </sst>
 </file>
@@ -1057,8 +1057,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B9376D30-AA93-47B8-A013-E886A455A1C7}">
   <dimension ref="A1:I41"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A35" zoomScale="87" workbookViewId="0">
-      <selection activeCell="B51" sqref="B51"/>
+    <sheetView tabSelected="1" zoomScale="87" workbookViewId="0">
+      <selection activeCell="B26" sqref="B26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1622,7 +1622,7 @@
         <v>15</v>
       </c>
       <c r="I19" s="3" t="s">
-        <v>206</v>
+        <v>203</v>
       </c>
     </row>
     <row r="20" spans="1:9" x14ac:dyDescent="0.3">
@@ -1804,7 +1804,7 @@
         <v>63</v>
       </c>
       <c r="B26" s="3" t="s">
-        <v>158</v>
+        <v>206</v>
       </c>
       <c r="C26" s="3" t="s">
         <v>156</v>
@@ -1833,10 +1833,10 @@
         <v>62</v>
       </c>
       <c r="B27" s="3" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="C27" s="3" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="D27" s="3" t="s">
         <v>139</v>
@@ -1845,7 +1845,7 @@
         <v>33</v>
       </c>
       <c r="F27" s="3" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="G27" s="3" t="s">
         <v>144</v>
@@ -1854,7 +1854,7 @@
         <v>15</v>
       </c>
       <c r="I27" s="3" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
     </row>
     <row r="28" spans="1:9" x14ac:dyDescent="0.3">
@@ -1862,10 +1862,10 @@
         <v>61</v>
       </c>
       <c r="B28" s="3" t="s">
-        <v>165</v>
+        <v>204</v>
       </c>
       <c r="C28" s="3" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="D28" s="3" t="s">
         <v>139</v>
@@ -1883,7 +1883,7 @@
         <v>15</v>
       </c>
       <c r="I28" s="3" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
     </row>
     <row r="29" spans="1:9" x14ac:dyDescent="0.3">
@@ -1891,10 +1891,10 @@
         <v>60</v>
       </c>
       <c r="B29" s="3" t="s">
-        <v>168</v>
+        <v>205</v>
       </c>
       <c r="C29" s="3" t="s">
-        <v>166</v>
+        <v>164</v>
       </c>
       <c r="D29" s="3" t="s">
         <v>139</v>
@@ -1912,7 +1912,7 @@
         <v>15</v>
       </c>
       <c r="I29" s="3" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
     </row>
     <row r="30" spans="1:9" x14ac:dyDescent="0.3">
@@ -1920,10 +1920,10 @@
         <v>59</v>
       </c>
       <c r="B30" s="3" t="s">
-        <v>170</v>
+        <v>167</v>
       </c>
       <c r="C30" s="3" t="s">
-        <v>169</v>
+        <v>166</v>
       </c>
       <c r="D30" s="3" t="s">
         <v>139</v>
@@ -1949,19 +1949,19 @@
         <v>58</v>
       </c>
       <c r="B31" s="3" t="s">
-        <v>175</v>
+        <v>172</v>
       </c>
       <c r="C31" s="3" t="s">
-        <v>171</v>
+        <v>168</v>
       </c>
       <c r="D31" s="3" t="s">
         <v>139</v>
       </c>
       <c r="E31" s="3" t="s">
-        <v>172</v>
+        <v>169</v>
       </c>
       <c r="F31" s="3" t="s">
-        <v>173</v>
+        <v>170</v>
       </c>
       <c r="G31" s="3" t="s">
         <v>144</v>
@@ -1970,7 +1970,7 @@
         <v>15</v>
       </c>
       <c r="I31" s="3" t="s">
-        <v>174</v>
+        <v>171</v>
       </c>
     </row>
     <row r="32" spans="1:9" x14ac:dyDescent="0.3">
@@ -1978,10 +1978,10 @@
         <v>57</v>
       </c>
       <c r="B32" s="3" t="s">
-        <v>178</v>
+        <v>175</v>
       </c>
       <c r="C32" s="3" t="s">
-        <v>176</v>
+        <v>173</v>
       </c>
       <c r="D32" s="3" t="s">
         <v>140</v>
@@ -1990,7 +1990,7 @@
         <v>145</v>
       </c>
       <c r="F32" s="3" t="s">
-        <v>177</v>
+        <v>174</v>
       </c>
       <c r="G32" s="3" t="s">
         <v>148</v>
@@ -1999,7 +1999,7 @@
         <v>15</v>
       </c>
       <c r="I32" s="3" t="s">
-        <v>179</v>
+        <v>176</v>
       </c>
     </row>
     <row r="33" spans="1:9" x14ac:dyDescent="0.3">
@@ -2007,10 +2007,10 @@
         <v>56</v>
       </c>
       <c r="B33" s="3" t="s">
-        <v>181</v>
+        <v>178</v>
       </c>
       <c r="C33" s="3" t="s">
-        <v>180</v>
+        <v>177</v>
       </c>
       <c r="D33" s="3" t="s">
         <v>140</v>
@@ -2036,10 +2036,10 @@
         <v>55</v>
       </c>
       <c r="B34" s="3" t="s">
-        <v>184</v>
+        <v>181</v>
       </c>
       <c r="C34" s="3" t="s">
-        <v>182</v>
+        <v>179</v>
       </c>
       <c r="D34" s="3" t="s">
         <v>140</v>
@@ -2057,7 +2057,7 @@
         <v>15</v>
       </c>
       <c r="I34" s="3" t="s">
-        <v>183</v>
+        <v>180</v>
       </c>
     </row>
     <row r="35" spans="1:9" x14ac:dyDescent="0.3">
@@ -2065,10 +2065,10 @@
         <v>54</v>
       </c>
       <c r="B35" s="3" t="s">
-        <v>187</v>
+        <v>184</v>
       </c>
       <c r="C35" s="3" t="s">
-        <v>185</v>
+        <v>182</v>
       </c>
       <c r="D35" s="3" t="s">
         <v>140</v>
@@ -2077,7 +2077,7 @@
         <v>19</v>
       </c>
       <c r="F35" s="3" t="s">
-        <v>186</v>
+        <v>183</v>
       </c>
       <c r="G35" s="3" t="s">
         <v>148</v>
@@ -2094,10 +2094,10 @@
         <v>53</v>
       </c>
       <c r="B36" s="3" t="s">
-        <v>190</v>
+        <v>187</v>
       </c>
       <c r="C36" s="3" t="s">
-        <v>188</v>
+        <v>185</v>
       </c>
       <c r="D36" s="3" t="s">
         <v>140</v>
@@ -2115,7 +2115,7 @@
         <v>15</v>
       </c>
       <c r="I36" s="3" t="s">
-        <v>189</v>
+        <v>186</v>
       </c>
     </row>
     <row r="37" spans="1:9" x14ac:dyDescent="0.3">
@@ -2123,10 +2123,10 @@
         <v>52</v>
       </c>
       <c r="B37" s="3" t="s">
-        <v>193</v>
+        <v>190</v>
       </c>
       <c r="C37" s="3" t="s">
-        <v>191</v>
+        <v>188</v>
       </c>
       <c r="D37" s="3" t="s">
         <v>140</v>
@@ -2135,7 +2135,7 @@
         <v>33</v>
       </c>
       <c r="F37" s="3" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="G37" s="3" t="s">
         <v>148</v>
@@ -2144,7 +2144,7 @@
         <v>15</v>
       </c>
       <c r="I37" s="3" t="s">
-        <v>192</v>
+        <v>189</v>
       </c>
     </row>
     <row r="38" spans="1:9" x14ac:dyDescent="0.3">
@@ -2152,10 +2152,10 @@
         <v>51</v>
       </c>
       <c r="B38" s="3" t="s">
-        <v>196</v>
+        <v>193</v>
       </c>
       <c r="C38" s="3" t="s">
-        <v>194</v>
+        <v>191</v>
       </c>
       <c r="D38" s="3" t="s">
         <v>140</v>
@@ -2173,7 +2173,7 @@
         <v>15</v>
       </c>
       <c r="I38" s="3" t="s">
-        <v>195</v>
+        <v>192</v>
       </c>
     </row>
     <row r="39" spans="1:9" x14ac:dyDescent="0.3">
@@ -2181,10 +2181,10 @@
         <v>50</v>
       </c>
       <c r="B39" s="3" t="s">
-        <v>199</v>
+        <v>196</v>
       </c>
       <c r="C39" s="3" t="s">
-        <v>197</v>
+        <v>194</v>
       </c>
       <c r="D39" s="3" t="s">
         <v>140</v>
@@ -2202,7 +2202,7 @@
         <v>15</v>
       </c>
       <c r="I39" s="3" t="s">
-        <v>198</v>
+        <v>195</v>
       </c>
     </row>
     <row r="40" spans="1:9" x14ac:dyDescent="0.3">
@@ -2210,10 +2210,10 @@
         <v>49</v>
       </c>
       <c r="B40" s="3" t="s">
-        <v>202</v>
+        <v>199</v>
       </c>
       <c r="C40" s="3" t="s">
-        <v>200</v>
+        <v>197</v>
       </c>
       <c r="D40" s="3" t="s">
         <v>140</v>
@@ -2231,7 +2231,7 @@
         <v>15</v>
       </c>
       <c r="I40" s="3" t="s">
-        <v>201</v>
+        <v>198</v>
       </c>
     </row>
     <row r="41" spans="1:9" x14ac:dyDescent="0.3">
@@ -2239,19 +2239,19 @@
         <v>48</v>
       </c>
       <c r="B41" s="3" t="s">
-        <v>205</v>
+        <v>202</v>
       </c>
       <c r="C41" s="3" t="s">
-        <v>203</v>
+        <v>200</v>
       </c>
       <c r="D41" s="3" t="s">
         <v>140</v>
       </c>
       <c r="E41" s="3" t="s">
-        <v>172</v>
+        <v>169</v>
       </c>
       <c r="F41" s="3" t="s">
-        <v>173</v>
+        <v>170</v>
       </c>
       <c r="G41" s="3" t="s">
         <v>148</v>
@@ -2260,7 +2260,7 @@
         <v>15</v>
       </c>
       <c r="I41" s="3" t="s">
-        <v>204</v>
+        <v>201</v>
       </c>
     </row>
   </sheetData>

</xml_diff>